<commit_message>
viet_nam codebook correction and working script 3
</commit_message>
<xml_diff>
--- a/samples/viet_nam2009/metadata/variables.metadata.manuallyedited.xlsx
+++ b/samples/viet_nam2009/metadata/variables.metadata.manuallyedited.xlsx
@@ -979,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1508,7 +1508,9 @@
       <c r="B9" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2">
+        <v>234</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>181</v>
       </c>

</xml_diff>